<commit_message>
Le menu est just
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Journal_de_bord.xlsx
+++ b/Doccument_théorique/Journal_de_bord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EAD548-540A-49B0-8027-83F717F9F409}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4695C1-66F2-4007-AD74-D7F10CD9ED96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14244" yWindow="1524" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>VIP</t>
+  </si>
+  <si>
+    <t>Finalisation de la grille</t>
   </si>
 </sst>
 </file>
@@ -97,7 +100,7 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Evénement"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="VIP"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -401,7 +404,7 @@
   <dimension ref="B3:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,8 +427,12 @@
       </c>
     </row>
     <row r="4" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="1">
+        <v>44265</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>

</xml_diff>

<commit_message>
Enregistre le score dans un fichier txt
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Journal_de_bord.xlsx
+++ b/Doccument_théorique/Journal_de_bord.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4695C1-66F2-4007-AD74-D7F10CD9ED96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7E34C6-4D1A-493D-A5EA-610DB3E80972}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14244" yWindow="1524" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>Finalisation de la grille</t>
+  </si>
+  <si>
+    <t>Enregistement du score</t>
+  </si>
+  <si>
+    <t>Arthru Bottemanne</t>
   </si>
 </sst>
 </file>
@@ -404,7 +410,7 @@
   <dimension ref="B3:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,8 +441,15 @@
       </c>
     </row>
     <row r="5" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
+      <c r="B5" s="1">
+        <v>44280</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>

</xml_diff>